<commit_message>
Updates to costs of fuel switching
</commit_message>
<xml_diff>
--- a/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
+++ b/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\United States\US_model\InputData\indst\CtIEPpUESoS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\indst\CtIEPpUESoS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BE47DD4-C2F7-40BB-833C-97C27A2092C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="early retirement" sheetId="4" r:id="rId2"/>
     <sheet name="cogen and WHR + eqpt stds" sheetId="6" r:id="rId3"/>
-    <sheet name="substitute fuels for coal" sheetId="5" r:id="rId4"/>
+    <sheet name="fuel type shifting" sheetId="5" r:id="rId4"/>
     <sheet name="CtIEPpUESoS" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,8 +36,51 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Gabe Mantegna</author>
+  </authors>
+  <commentList>
+    <comment ref="C43" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Gabe Mantegna:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Hydrogen boilers estimated to cost 1.5x the cost of building a natural gas boiler by mid-century when manufacturing capacity has scaled </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="128">
   <si>
     <t>Source:</t>
   </si>
@@ -109,9 +154,6 @@
     <t>Investment per Unit Annual Energy Savings ($/BTU)</t>
   </si>
   <si>
-    <t>Investment per Unit Energy Converted ($/BTU)</t>
-  </si>
-  <si>
     <t>Rocky Mountain Institute</t>
   </si>
   <si>
@@ -157,9 +199,6 @@
     <t>cogeneration and waste heat recovery</t>
   </si>
   <si>
-    <t>substitute other fuels for coal</t>
-  </si>
-  <si>
     <t>eqpt efficiency stds</t>
   </si>
   <si>
@@ -169,18 +208,9 @@
     <t>early retirement of equipment</t>
   </si>
   <si>
-    <t>Substitute Other Fuels for Coal</t>
-  </si>
-  <si>
     <t>Notes:</t>
   </si>
   <si>
-    <t>For the "subsitute other fuels for coal" policy, the cost is per unit of energy shifted from coal to</t>
-  </si>
-  <si>
-    <t>another fuel type, not per unit of energy saved.</t>
-  </si>
-  <si>
     <t>achieves this energy savings/shifting annually.</t>
   </si>
   <si>
@@ -286,9 +316,6 @@
     <t>2010 to 2012, RMI and Babcock and Wilcox</t>
   </si>
   <si>
-    <t>substitute other fuels for natural gas</t>
-  </si>
-  <si>
     <t>This variable supports time series data for adaptation to other regions, but as of EPS 1.5.0, we</t>
   </si>
   <si>
@@ -340,60 +367,120 @@
     <t>MMBtu/yr</t>
   </si>
   <si>
-    <t>Investment per Unit Energy Converted</t>
-  </si>
-  <si>
-    <t>$/btu</t>
-  </si>
-  <si>
-    <t>Btu/yr</t>
-  </si>
-  <si>
-    <t>substitute other fuels for coal and gas: cost of new electric capacity</t>
-  </si>
-  <si>
-    <t>Table 17. Capital and Fuel Cost Comparison of 100-Boiler Horsepower Natural Gas and Electric Steam Boilers (pg 64)</t>
-  </si>
-  <si>
-    <t>NREL</t>
-  </si>
-  <si>
-    <t>"Electrification Futures Study: End-Use Electric Technology Cost and Performance Projections through 2050"</t>
-  </si>
-  <si>
-    <t>https://www.nrel.gov/docs/fy18osti/70485.pdf</t>
-  </si>
-  <si>
-    <t>We estimate the cost of installing new electric-fired boilers using E3's methodology "Achieving Carbon Neutrality in California (Revised Report): 2045 Abatement Cost Estimates"</t>
-  </si>
-  <si>
-    <t>https://www.ethree.com/achieving-carbon-neutrality-in-california-e3-presents-draft-report-at-california-air-resources-board-public-workshop/</t>
-  </si>
-  <si>
-    <t>substitute other fuels for coal and gas: cost of new electric capacity - methodology</t>
-  </si>
-  <si>
     <t>E3</t>
   </si>
   <si>
     <t>"Achieving Carbon Neutrality in California (Revised Report): 2045 Abatement Cost Estimates"</t>
+  </si>
+  <si>
+    <t>https://ww2.arb.ca.gov/sites/default/files/2020-09/e3_cn_draft_report_supp_data_aug2020.xlsx</t>
+  </si>
+  <si>
+    <t>fuel type shifting</t>
+  </si>
+  <si>
+    <t>Fuel Type Shifting</t>
+  </si>
+  <si>
+    <t>Electric Boiler Conversion</t>
+  </si>
+  <si>
+    <t>Hydrogen Boiler Conversion</t>
+  </si>
+  <si>
+    <t>General Inputs</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Equipment Lifetime</t>
+  </si>
+  <si>
+    <t>yr</t>
+  </si>
+  <si>
+    <t>Discount Rate</t>
+  </si>
+  <si>
+    <t>Natural Gas Price</t>
+  </si>
+  <si>
+    <t>$/MMBtu</t>
+  </si>
+  <si>
+    <t>Synthetic Natural Gas Price (Conservative)</t>
+  </si>
+  <si>
+    <t>Synthetic Natural Gas Price (Optimistic)</t>
+  </si>
+  <si>
+    <t>Hydrogen Price (Conservative)</t>
+  </si>
+  <si>
+    <t>Hydrogen Price (Optimistic)</t>
+  </si>
+  <si>
+    <t>Hydrogen Storage and Delivery Cost</t>
+  </si>
+  <si>
+    <t>$/MMBTU</t>
+  </si>
+  <si>
+    <t>Hydrogen Boiler Conservative</t>
+  </si>
+  <si>
+    <t>Hydrogen Boiler Optimistic</t>
+  </si>
+  <si>
+    <t>Natural Gas Boiler Pice</t>
+  </si>
+  <si>
+    <t>H2 Boiler Price</t>
+  </si>
+  <si>
+    <t>H2 Boiler Efficiency</t>
+  </si>
+  <si>
+    <t>Electricity Emissions Intensity</t>
+  </si>
+  <si>
+    <t>kg CO2e/kWh</t>
+  </si>
+  <si>
+    <t>Natural Gas Emissions Intensity</t>
+  </si>
+  <si>
+    <t>kg CO2e/MMBtu</t>
+  </si>
+  <si>
+    <t>Natural Gas Boiler</t>
+  </si>
+  <si>
+    <t>Investment per Unit Energy Converted in First Year ($/BTU)</t>
+  </si>
+  <si>
+    <t>For fuel type shifting we take an average of electric boiler conversion and hydrogen boiler conversion.</t>
+  </si>
+  <si>
+    <t>We assume the majority of energy and costs will be from boiler conversion instead of process heaters.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="0.0E+00"/>
     <numFmt numFmtId="168" formatCode="#,##0.000"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,8 +543,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,14 +589,8 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -547,17 +649,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -579,10 +670,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -646,27 +737,30 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="10" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="10" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="5" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="9" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="5" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Body: normal cell" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Comma" xfId="9" builtinId="3"/>
+    <cellStyle name="Body: normal cell" xfId="6"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="4"/>
+    <cellStyle name="Footnotes: top row" xfId="8"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="10" builtinId="10"/>
-    <cellStyle name="Parent row" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Table title" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Parent row" xfId="7"/>
+    <cellStyle name="Percent" xfId="10" builtinId="5"/>
+    <cellStyle name="Table title" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -734,6 +828,79 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover"/>
+      <sheetName val="Summary"/>
+      <sheetName val="Electricity Decarbonization"/>
+      <sheetName val="Industry Elec. - Boilers"/>
+      <sheetName val="Industry Elec. - Process Heat"/>
+      <sheetName val="Industry CCS - Process Heat"/>
+      <sheetName val="Industry Hydrogen &amp; SNG"/>
+      <sheetName val="MDV &amp; HDV Decarbonization"/>
+      <sheetName val="DAC &amp; BECCS"/>
+      <sheetName val="Fuel Costs - PATHWAYS"/>
+      <sheetName val="Emission Factors - PATHWAYS"/>
+      <sheetName val="Constants"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9">
+        <row r="19">
+          <cell r="E19">
+            <v>5.6539999999999999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="10">
+        <row r="7">
+          <cell r="E7">
+            <v>1.7765038912431299</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="E19">
+            <v>50.07</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="11">
+        <row r="5">
+          <cell r="D5">
+            <v>1055.06</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="D6">
+            <v>3600000</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27">
+            <v>229.59399999999999</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>251.107</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -812,23 +979,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -864,23 +1014,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1056,11 +1189,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1203,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1078,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1108,12 +1241,12 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,214 +1256,184 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>2011</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="5">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="25" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="25"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-    </row>
-    <row r="40" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="25"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+    </row>
+    <row r="33" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>48</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="25" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="25">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="B52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="26">
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="25" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="25">
-        <v>0.98699999999999999</v>
-      </c>
-      <c r="B59" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="26">
-        <v>1.0549999999999999</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="25" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B21" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B21" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
@@ -1338,7 +1441,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1488,14 +1591,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1511,7 +1614,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1519,13 +1622,13 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B3" s="10"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B4" s="21">
         <f>2.4*10^15</f>
@@ -1534,7 +1637,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B5" s="21">
         <f>2.3*10^15</f>
@@ -1546,32 +1649,32 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1579,47 +1682,47 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -1628,21 +1731,21 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B25" s="17">
         <v>114</v>
@@ -1661,7 +1764,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B26" s="17">
         <v>114</v>
@@ -1686,7 +1789,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="18"/>
@@ -1694,7 +1797,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B29" s="23">
         <f>E25/B4</f>
@@ -1705,7 +1808,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B30" s="23">
         <f>E26/B5</f>
@@ -1722,11 +1825,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,148 +1841,474 @@
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="31">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="32">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="33">
+        <f>'[1]Fuel Costs - PATHWAYS'!$E$19*([1]Constants!$C$33/[1]Constants!$C$27)*[1]Constants!$D$5/1000</f>
+        <v>6.5242598122280206</v>
+      </c>
+      <c r="D10" s="38"/>
+    </row>
+    <row r="11" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="39">
+        <f>'[1]Emission Factors - PATHWAYS'!$E$7/10^9*[1]Constants!$D$6</f>
+        <v>6.3954140084752677E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="39">
+        <f>'[1]Emission Factors - PATHWAYS'!$E$19*([1]Constants!$D$5/1000)</f>
+        <v>52.826854199999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="34">
+        <v>53860</v>
+      </c>
+      <c r="D16" s="34">
+        <v>87540</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="32">
+        <v>1</v>
+      </c>
+      <c r="D17" s="35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="36">
+        <v>3.3475000000000001</v>
+      </c>
+      <c r="D18" s="36">
+        <v>3.3475000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="C19" s="37">
+        <v>5280</v>
+      </c>
+      <c r="D19" s="37">
+        <v>5280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="B20" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="37">
+        <f>C18*C19</f>
+        <v>17674.8</v>
+      </c>
+      <c r="D20" s="37">
+        <f>D18*D19</f>
+        <v>17674.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="14"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <f>C16/(C20*10^6)</f>
+        <v>3.047276348247222E-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="31">
+        <v>25</v>
+      </c>
+      <c r="D31" s="25"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="D32" s="25"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="33">
+        <f>'[1]Fuel Costs - PATHWAYS'!$E$19*([1]Constants!$C$33/[1]Constants!$C$27)*[1]Constants!$D$5/1000</f>
+        <v>6.5242598122280206</v>
+      </c>
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="34">
+        <v>44</v>
+      </c>
+      <c r="D34" s="25"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="34">
+        <v>34</v>
+      </c>
+      <c r="D35" s="25"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="34">
+        <v>21</v>
+      </c>
+      <c r="D36" s="25"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="34">
+        <v>15</v>
+      </c>
+      <c r="D37" s="25"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="34">
+        <v>4</v>
+      </c>
+      <c r="D38" s="25"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="31" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="30" t="s">
+      <c r="C42" s="34">
+        <v>87540</v>
+      </c>
+      <c r="D42" s="34">
+        <v>87540</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="34">
+        <f>C42*1.5</f>
+        <v>131310</v>
+      </c>
+      <c r="D43" s="34">
+        <v>87540</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="32">
+        <f>D44</f>
+        <v>0.8</v>
+      </c>
+      <c r="D44" s="35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="36">
+        <v>3.3475000000000001</v>
+      </c>
+      <c r="D45" s="36">
+        <v>3.3475000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="37">
+        <v>5280</v>
+      </c>
+      <c r="D46" s="37">
+        <v>5280</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="31">
-        <v>53860</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="33">
-        <v>3.3475000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="34">
-        <v>5280</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="C11" s="34">
-        <f>C9*C10</f>
+      <c r="C47" s="37">
+        <f>C45*C46</f>
         <v>17674.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="34">
-        <f>C11*10^6</f>
-        <v>17674800000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="36">
-        <f>C7/(C11*10^6)</f>
-        <v>3.047276348247222E-6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="14"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <f>C13</f>
-        <v>3.047276348247222E-6</v>
+      <c r="D47" s="37">
+        <f>D45*D46</f>
+        <v>17674.8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="19">
+        <f>AVERAGE(C43:D43)/(AVERAGE(C47:D47)*10^6)</f>
+        <v>6.1910177201439334E-6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,7 +2319,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B1" s="27">
         <v>2018</v>
@@ -1994,10 +2423,10 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="20">
-        <f>'early retirement'!A20*About!$A$59</f>
+        <f>'early retirement'!A20*About!$A$52</f>
         <v>1.4243732995275992E-4</v>
       </c>
       <c r="C2" s="20">
@@ -2009,7 +2438,7 @@
         <v>1.4243732995275992E-4</v>
       </c>
       <c r="E2" s="20">
-        <f t="shared" ref="E2:AH8" si="0">$B2</f>
+        <f t="shared" ref="E2:AH7" si="0">$B2</f>
         <v>1.4243732995275992E-4</v>
       </c>
       <c r="F2" s="20">
@@ -2131,13 +2560,13 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="28">
-        <f t="shared" ref="C3:R8" si="1">$B3</f>
+        <f t="shared" ref="C3:R7" si="1">$B3</f>
         <v>0</v>
       </c>
       <c r="D3" s="28">
@@ -2267,10 +2696,10 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="20">
-        <f>'cogen and WHR + eqpt stds'!B29*About!$A$60</f>
+        <f>'cogen and WHR + eqpt stds'!B29*About!$A$53</f>
         <v>2.4092251461988303E-5</v>
       </c>
       <c r="C4" s="20">
@@ -2404,10 +2833,10 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="20">
-        <f>'cogen and WHR + eqpt stds'!B30*About!$A$60</f>
+        <f>'cogen and WHR + eqpt stds'!B30*About!$A$53</f>
         <v>5.7135774218154072E-6</v>
       </c>
       <c r="C5" s="20">
@@ -2541,410 +2970,273 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="B6" s="20">
-        <f>'substitute fuels for coal'!A17*About!$A$60</f>
-        <v>3.214876547400819E-6</v>
+        <f>AVERAGE('fuel type shifting'!A24,'fuel type shifting'!A50)*About!$A$53</f>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="C6" s="20">
         <f t="shared" si="1"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="D6" s="20">
         <f t="shared" si="1"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="E6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="F6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="G6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="H6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="I6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="J6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="K6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="L6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="M6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="N6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="O6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="P6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="Q6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="R6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="S6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="T6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="U6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="V6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="W6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="X6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="Y6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="Z6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="AA6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="AB6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="AC6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="AD6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="AE6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="AF6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="AG6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
+        <v>4.8732001210763347E-6</v>
       </c>
       <c r="AH6" s="20">
         <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="20">
-        <f>B6</f>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="C7" s="20">
+        <v>4.8732001210763347E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="28">
         <f t="shared" si="1"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="D7" s="20">
+        <v>0</v>
+      </c>
+      <c r="D7" s="28">
         <f t="shared" si="1"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="E7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="F7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="G7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="H7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="I7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="J7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="K7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="L7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="M7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="N7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="O7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="P7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="Q7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="R7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="S7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="T7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="U7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="V7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="W7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="X7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="Y7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="Z7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="AA7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="AB7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="AC7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="AD7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="AE7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="AF7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="AG7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-      <c r="AH7" s="20">
-        <f t="shared" si="0"/>
-        <v>3.214876547400819E-6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D8" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AG8" s="28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AH8" s="28">
+        <v>0</v>
+      </c>
+      <c r="E7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH7" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Finish disaggregating industrial heat by temperature (#196)
</commit_message>
<xml_diff>
--- a/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
+++ b/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
@@ -1,27 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\indst\CtIEPpUESoS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\indst\CtIEPpUESoS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F874FF-DD42-4208-ACE1-EC7ADF39DF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4"/>
+    <workbookView xWindow="16425" yWindow="1830" windowWidth="25815" windowHeight="19845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="early retirement" sheetId="4" r:id="rId2"/>
     <sheet name="cogen and WHR + eqpt stds" sheetId="6" r:id="rId3"/>
-    <sheet name="fuel type shifting" sheetId="5" r:id="rId4"/>
-    <sheet name="CtIEPpUESoS" sheetId="3" r:id="rId5"/>
+    <sheet name="med and high temp fuel shifting" sheetId="5" r:id="rId4"/>
+    <sheet name="low temp fuel type shifting" sheetId="8" r:id="rId5"/>
+    <sheet name="CtIEPpUESoS" sheetId="3" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,6 +33,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,12 +41,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gabe Mantegna</author>
   </authors>
   <commentList>
-    <comment ref="C43" authorId="0" shapeId="0">
+    <comment ref="C43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="140">
   <si>
     <t>Source:</t>
   </si>
@@ -464,12 +468,48 @@
   </si>
   <si>
     <t>We assume the majority of energy and costs will be from boiler conversion instead of process heaters.</t>
+  </si>
+  <si>
+    <t>med and high temp fuel type shifting</t>
+  </si>
+  <si>
+    <t>low temp fuel type shifting</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Low temp fuel shifting is always electrification via heat pumps.</t>
+  </si>
+  <si>
+    <t>Heat pump efficiency varies with temperature increase.  When increasing temperature to 100 C (from room temp), heat pump efficiency is often around 2.5 COP.</t>
+  </si>
+  <si>
+    <t>Temp Increase (°C)</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Arpagaus, Cordin et al.</t>
+  </si>
+  <si>
+    <t>High Temperature Heat Pumps: Market Overview, State of the Art, Research Status, Refrigerants, and Application Potentials</t>
+  </si>
+  <si>
+    <t>https://docs.lib.purdue.edu/cgi/viewcontent.cgi?article=2875&amp;context=iracc</t>
+  </si>
+  <si>
+    <t>Assumed COP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
@@ -565,7 +605,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -587,6 +627,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -673,7 +719,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -748,19 +794,24 @@
     <xf numFmtId="3" fontId="0" fillId="4" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="5" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Body: normal cell" xfId="6"/>
+    <cellStyle name="Body: normal cell" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="4"/>
-    <cellStyle name="Footnotes: top row" xfId="8"/>
-    <cellStyle name="Header: bottom row" xfId="5"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Parent row" xfId="7"/>
+    <cellStyle name="Parent row" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
-    <cellStyle name="Table title" xfId="3"/>
+    <cellStyle name="Table title" xfId="3" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,6 +824,2351 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[2]Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="9"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="31750">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[2]Sheet1!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>56.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>60.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>84.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[2]Sheet1!$B$2:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.69</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CB75-4B35-AE4F-D1B8F04D2988}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1808965472"/>
+        <c:axId val="1808962144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1808965472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1808962144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1808962144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1808965472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800"/>
+              <a:t>Industrial Heat Pump Efficiency vs. Delivered</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="0"/>
+              <a:t> Temperature Increase</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[2]Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>COP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[2]Sheet1!$A$2:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>56.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>60.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>84.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[2]Sheet1!$B$2:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.69</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2.19</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.98</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.58</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8896-4A4E-A4E1-3559C9BE4B76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2005302688"/>
+        <c:axId val="2005298112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2005302688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Temperature Increase (°C)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2005298112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2005298112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Coefficient of Performance (COP)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.1590044939753746E-3"/>
+              <c:y val="0.24265854338040146"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2005302688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -830,6 +3226,137 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>20292</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>168551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>477493</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>69684</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DE96396-2DDB-450C-B51F-375BE16A15A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2639667" y="168551"/>
+          <a:ext cx="7772401" cy="7140133"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>329852</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>151881</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>229843</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>130450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56B4AFDD-A87E-433C-A5DF-232773DD5ABA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2278</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>156127</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>236482</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>118027</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7312B4DD-5BBD-4C5E-A2B4-400ED73554D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -895,6 +3422,345 @@
         <row r="33">
           <cell r="C33">
             <v>251.107</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>COP</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>25</v>
+          </cell>
+          <cell r="B2">
+            <v>5.77</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>30</v>
+          </cell>
+          <cell r="B3">
+            <v>4.99</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>35</v>
+          </cell>
+          <cell r="B4">
+            <v>4.01</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>40</v>
+          </cell>
+          <cell r="B5">
+            <v>4.71</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>40</v>
+          </cell>
+          <cell r="B6">
+            <v>4.25</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>40</v>
+          </cell>
+          <cell r="B7">
+            <v>4.05</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>40</v>
+          </cell>
+          <cell r="B8">
+            <v>3.95</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>40</v>
+          </cell>
+          <cell r="B9">
+            <v>3.66</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>40</v>
+          </cell>
+          <cell r="B10">
+            <v>3.39</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>45</v>
+          </cell>
+          <cell r="B11">
+            <v>4.9800000000000004</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>45.2</v>
+          </cell>
+          <cell r="B12">
+            <v>3.99</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>50</v>
+          </cell>
+          <cell r="B13">
+            <v>4.0999999999999996</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>50.8</v>
+          </cell>
+          <cell r="B14">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>50</v>
+          </cell>
+          <cell r="B15">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>50</v>
+          </cell>
+          <cell r="B16">
+            <v>3.6</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>50</v>
+          </cell>
+          <cell r="B17">
+            <v>3.35</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>50</v>
+          </cell>
+          <cell r="B18">
+            <v>3.1</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>50</v>
+          </cell>
+          <cell r="B19">
+            <v>2.98</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>55</v>
+          </cell>
+          <cell r="B20">
+            <v>3.5</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>55</v>
+          </cell>
+          <cell r="B21">
+            <v>2.7</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>56.4</v>
+          </cell>
+          <cell r="B22">
+            <v>3.6</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>60.2</v>
+          </cell>
+          <cell r="B23">
+            <v>4.5</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>60</v>
+          </cell>
+          <cell r="B24">
+            <v>2.89</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>60</v>
+          </cell>
+          <cell r="B25">
+            <v>2.75</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>60</v>
+          </cell>
+          <cell r="B26">
+            <v>2.06</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>63.2</v>
+          </cell>
+          <cell r="B27">
+            <v>2.69</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>61.4</v>
+          </cell>
+          <cell r="B28">
+            <v>3.45</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>65</v>
+          </cell>
+          <cell r="B29">
+            <v>3.1</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>70</v>
+          </cell>
+          <cell r="B30">
+            <v>2.6</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>75</v>
+          </cell>
+          <cell r="B31">
+            <v>2.7</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>75</v>
+          </cell>
+          <cell r="B32">
+            <v>2.37</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>80</v>
+          </cell>
+          <cell r="B33">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>84.7</v>
+          </cell>
+          <cell r="B34">
+            <v>2.2999999999999998</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>90</v>
+          </cell>
+          <cell r="B35">
+            <v>1.98</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>95</v>
+          </cell>
+          <cell r="B36">
+            <v>2.48</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>95</v>
+          </cell>
+          <cell r="B37">
+            <v>1.98</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>100</v>
+          </cell>
+          <cell r="B38">
+            <v>1.69</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>105</v>
+          </cell>
+          <cell r="B39">
+            <v>2.19</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>115</v>
+          </cell>
+          <cell r="B40">
+            <v>1.98</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>130</v>
+          </cell>
+          <cell r="B41">
+            <v>1.58</v>
           </cell>
         </row>
       </sheetData>
@@ -979,6 +3845,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1014,6 +3897,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1189,12 +4089,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1431,9 +4329,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
-    <hyperlink ref="B21" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B21" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
@@ -1441,7 +4339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1591,14 +4489,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1825,11 +4723,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2301,15 +5199,412 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70154B78-0E9B-4A9B-9D3C-65AF6790BABC}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:B54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" style="25" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="41">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
+        <v>25</v>
+      </c>
+      <c r="B15" s="25">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
+        <v>30</v>
+      </c>
+      <c r="B16" s="25">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
+        <v>35</v>
+      </c>
+      <c r="B17" s="25">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
+        <v>40</v>
+      </c>
+      <c r="B18" s="25">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
+        <v>40</v>
+      </c>
+      <c r="B19" s="25">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="25">
+        <v>40</v>
+      </c>
+      <c r="B20" s="25">
+        <v>4.05</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="25">
+        <v>40</v>
+      </c>
+      <c r="B21" s="25">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
+        <v>40</v>
+      </c>
+      <c r="B22" s="25">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="25">
+        <v>40</v>
+      </c>
+      <c r="B23" s="25">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="25">
+        <v>45</v>
+      </c>
+      <c r="B24" s="25">
+        <v>4.9800000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
+        <v>45.2</v>
+      </c>
+      <c r="B25" s="25">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="25">
+        <v>50</v>
+      </c>
+      <c r="B26" s="25">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="25">
+        <v>50.8</v>
+      </c>
+      <c r="B27" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>50</v>
+      </c>
+      <c r="B28" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="25">
+        <v>50</v>
+      </c>
+      <c r="B29" s="25">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="25">
+        <v>50</v>
+      </c>
+      <c r="B30" s="25">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="25">
+        <v>50</v>
+      </c>
+      <c r="B31" s="25">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="25">
+        <v>50</v>
+      </c>
+      <c r="B32" s="25">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="25">
+        <v>55</v>
+      </c>
+      <c r="B33" s="25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="25">
+        <v>55</v>
+      </c>
+      <c r="B34" s="25">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="25">
+        <v>56.4</v>
+      </c>
+      <c r="B35" s="25">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="25">
+        <v>60.2</v>
+      </c>
+      <c r="B36" s="25">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="25">
+        <v>60</v>
+      </c>
+      <c r="B37" s="25">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="25">
+        <v>60</v>
+      </c>
+      <c r="B38" s="25">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="25">
+        <v>60</v>
+      </c>
+      <c r="B39" s="25">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="25">
+        <v>63.2</v>
+      </c>
+      <c r="B40" s="25">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="25">
+        <v>61.4</v>
+      </c>
+      <c r="B41" s="25">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="25">
+        <v>65</v>
+      </c>
+      <c r="B42" s="25">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="25">
+        <v>70</v>
+      </c>
+      <c r="B43" s="25">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="25">
+        <v>75</v>
+      </c>
+      <c r="B44" s="25">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="25">
+        <v>75</v>
+      </c>
+      <c r="B45" s="25">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="25">
+        <v>80</v>
+      </c>
+      <c r="B46" s="25">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="25">
+        <v>84.7</v>
+      </c>
+      <c r="B47" s="25">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="25">
+        <v>90</v>
+      </c>
+      <c r="B48" s="25">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="25">
+        <v>95</v>
+      </c>
+      <c r="B49" s="25">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="25">
+        <v>95</v>
+      </c>
+      <c r="B50" s="25">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="25">
+        <v>100</v>
+      </c>
+      <c r="B51" s="25">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="25">
+        <v>105</v>
+      </c>
+      <c r="B52" s="25">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="25">
+        <v>115</v>
+      </c>
+      <c r="B53" s="25">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="25">
+        <v>130</v>
+      </c>
+      <c r="B54" s="25">
+        <v>1.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2438,7 +5733,7 @@
         <v>1.4243732995275992E-4</v>
       </c>
       <c r="E2" s="20">
-        <f t="shared" ref="E2:AH7" si="0">$B2</f>
+        <f t="shared" ref="E2:AH8" si="0">$B2</f>
         <v>1.4243732995275992E-4</v>
       </c>
       <c r="F2" s="20">
@@ -2566,7 +5861,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="28">
-        <f t="shared" ref="C3:R7" si="1">$B3</f>
+        <f t="shared" ref="C3:R8" si="1">$B3</f>
         <v>0</v>
       </c>
       <c r="D3" s="28">
@@ -2970,10 +6265,10 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="B6" s="20">
-        <f>AVERAGE('fuel type shifting'!A24,'fuel type shifting'!A50)*About!$A$53</f>
+        <f>AVERAGE('med and high temp fuel shifting'!A24,'med and high temp fuel shifting'!A50)*About!$A$53</f>
         <v>4.8732001210763347E-6</v>
       </c>
       <c r="C6" s="20">
@@ -3105,138 +6400,275 @@
         <v>4.8732001210763347E-6</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:34" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="42">
+        <f>B6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="C7" s="42">
+        <f>C6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="D7" s="42">
+        <f>D6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="E7" s="42">
+        <f>E6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="F7" s="42">
+        <f>F6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="G7" s="42">
+        <f>G6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="H7" s="42">
+        <f>H6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="I7" s="42">
+        <f>I6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="J7" s="42">
+        <f>J6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="K7" s="42">
+        <f>K6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="L7" s="42">
+        <f>L6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="M7" s="42">
+        <f>M6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="N7" s="42">
+        <f>N6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="O7" s="42">
+        <f>O6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="P7" s="42">
+        <f>P6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="Q7" s="42">
+        <f>Q6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="R7" s="42">
+        <f>R6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="S7" s="42">
+        <f>S6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="T7" s="42">
+        <f>T6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="U7" s="42">
+        <f>U6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="V7" s="42">
+        <f>V6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="W7" s="42">
+        <f>W6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="X7" s="42">
+        <f>X6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="Y7" s="42">
+        <f>Y6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="Z7" s="42">
+        <f>Z6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="AA7" s="42">
+        <f>AA6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="AB7" s="42">
+        <f>AB6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="AC7" s="42">
+        <f>AC6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="AD7" s="42">
+        <f>AD6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="AE7" s="42">
+        <f>AE6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="AF7" s="42">
+        <f>AF6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="AG7" s="42">
+        <f>AG6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+      <c r="AH7" s="42">
+        <f>AH6/'low temp fuel type shifting'!$B$6</f>
+        <v>1.9492800484305339E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C8" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D8" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O7" s="28">
+      <c r="O8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P7" s="28">
+      <c r="P8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="28">
+      <c r="Q8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R7" s="28">
+      <c r="R8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S7" s="28">
+      <c r="S8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T7" s="28">
+      <c r="T8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U7" s="28">
+      <c r="U8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V7" s="28">
+      <c r="V8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W7" s="28">
+      <c r="W8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X7" s="28">
+      <c r="X8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y7" s="28">
+      <c r="Y8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z7" s="28">
+      <c r="Z8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA7" s="28">
+      <c r="AA8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB7" s="28">
+      <c r="AB8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC7" s="28">
+      <c r="AC8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="28">
+      <c r="AD8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE7" s="28">
+      <c r="AE8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AF7" s="28">
+      <c r="AF8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AG7" s="28">
+      <c r="AG8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AH7" s="28">
+      <c r="AH8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Correction to heat pump cost data (#196)
</commit_message>
<xml_diff>
--- a/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
+++ b/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\indst\CtIEPpUESoS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD6D5E8-CD8E-4BF6-ADE5-BC3B2A24EAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4E9C2A-F4CA-4670-8026-422A565CD66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="465" windowWidth="24585" windowHeight="22005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10905" yWindow="780" windowWidth="15900" windowHeight="22005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,6 @@
     <sheet name="low temp fuel type shifting" sheetId="8" r:id="rId5"/>
     <sheet name="CtIEPpUESoS" sheetId="3" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -83,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="146">
   <si>
     <t>Source:</t>
   </si>
@@ -503,13 +500,31 @@
   </si>
   <si>
     <t>https://climate.emerson.com/documents/vilter-heat-pump-white-paper-en-us-5411194.pdf</t>
+  </si>
+  <si>
+    <t>This is the cost per unit heat delivered via heat pump.</t>
+  </si>
+  <si>
+    <t>We want the cost per unit energy saved or shifted.</t>
+  </si>
+  <si>
+    <t>Therefore, we need to take into account the difference in efficiency of heat use.</t>
+  </si>
+  <si>
+    <t>From variable indst/PIFURfE</t>
+  </si>
+  <si>
+    <t>Percent reduction in fuel use from switching from fossil fuels to heat pump is:</t>
+  </si>
+  <si>
+    <t>Therefore, the capital cost per unit energy saved (not per unit energy delivered) is:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
@@ -519,6 +534,7 @@
     <numFmt numFmtId="168" formatCode="#,##0.000"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
     <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="0.0%"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -611,7 +627,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -638,6 +654,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,7 +747,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -809,6 +831,8 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Body: normal cell" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -889,345 +913,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>COP</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>25</v>
-          </cell>
-          <cell r="B2">
-            <v>5.77</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>30</v>
-          </cell>
-          <cell r="B3">
-            <v>4.99</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>35</v>
-          </cell>
-          <cell r="B4">
-            <v>4.01</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>40</v>
-          </cell>
-          <cell r="B5">
-            <v>4.71</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>40</v>
-          </cell>
-          <cell r="B6">
-            <v>4.25</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>40</v>
-          </cell>
-          <cell r="B7">
-            <v>4.05</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>40</v>
-          </cell>
-          <cell r="B8">
-            <v>3.95</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>40</v>
-          </cell>
-          <cell r="B9">
-            <v>3.66</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>40</v>
-          </cell>
-          <cell r="B10">
-            <v>3.39</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>45</v>
-          </cell>
-          <cell r="B11">
-            <v>4.9800000000000004</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>45.2</v>
-          </cell>
-          <cell r="B12">
-            <v>3.99</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>50</v>
-          </cell>
-          <cell r="B13">
-            <v>4.0999999999999996</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>50.8</v>
-          </cell>
-          <cell r="B14">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>50</v>
-          </cell>
-          <cell r="B15">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>50</v>
-          </cell>
-          <cell r="B16">
-            <v>3.6</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>50</v>
-          </cell>
-          <cell r="B17">
-            <v>3.35</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>50</v>
-          </cell>
-          <cell r="B18">
-            <v>3.1</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>50</v>
-          </cell>
-          <cell r="B19">
-            <v>2.98</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>55</v>
-          </cell>
-          <cell r="B20">
-            <v>3.5</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>55</v>
-          </cell>
-          <cell r="B21">
-            <v>2.7</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>56.4</v>
-          </cell>
-          <cell r="B22">
-            <v>3.6</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>60.2</v>
-          </cell>
-          <cell r="B23">
-            <v>4.5</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>60</v>
-          </cell>
-          <cell r="B24">
-            <v>2.89</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>60</v>
-          </cell>
-          <cell r="B25">
-            <v>2.75</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>60</v>
-          </cell>
-          <cell r="B26">
-            <v>2.06</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>63.2</v>
-          </cell>
-          <cell r="B27">
-            <v>2.69</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>61.4</v>
-          </cell>
-          <cell r="B28">
-            <v>3.45</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>65</v>
-          </cell>
-          <cell r="B29">
-            <v>3.1</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>70</v>
-          </cell>
-          <cell r="B30">
-            <v>2.6</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>75</v>
-          </cell>
-          <cell r="B31">
-            <v>2.7</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>75</v>
-          </cell>
-          <cell r="B32">
-            <v>2.37</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>80</v>
-          </cell>
-          <cell r="B33">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>84.7</v>
-          </cell>
-          <cell r="B34">
-            <v>2.2999999999999998</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>90</v>
-          </cell>
-          <cell r="B35">
-            <v>1.98</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>95</v>
-          </cell>
-          <cell r="B36">
-            <v>2.48</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>95</v>
-          </cell>
-          <cell r="B37">
-            <v>1.98</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>100</v>
-          </cell>
-          <cell r="B38">
-            <v>1.69</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>105</v>
-          </cell>
-          <cell r="B39">
-            <v>2.19</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>115</v>
-          </cell>
-          <cell r="B40">
-            <v>1.98</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>130</v>
-          </cell>
-          <cell r="B41">
-            <v>1.58</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2685,9 +2370,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70154B78-0E9B-4A9B-9D3C-65AF6790BABC}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2770,9 +2457,50 @@
         <f>AVERAGE(C4:C6)</f>
         <v>900000</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="46">
         <f t="shared" si="0"/>
         <v>1.8903988741624482E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="45">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="43">
+        <f>D7*(1-A15)</f>
+        <v>6.1627003297695804E-6</v>
       </c>
     </row>
   </sheetData>
@@ -2789,9 +2517,7 @@
   </sheetPr>
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3592,136 +3318,136 @@
         <v>127</v>
       </c>
       <c r="B7" s="44">
-        <f>'low temp fuel type shifting'!D7</f>
-        <v>1.8903988741624482E-5</v>
+        <f>'low temp fuel type shifting'!A18</f>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="C7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="D7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="E7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="F7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="G7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="H7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="I7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="J7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="K7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="L7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="M7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="N7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="O7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="P7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="Q7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="R7" s="20">
         <f t="shared" si="1"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="S7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="T7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="U7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="V7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="W7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="X7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="Y7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="Z7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="AA7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="AB7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="AC7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="AD7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="AE7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="AF7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="AG7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
       <c r="AH7" s="20">
         <f t="shared" si="0"/>
-        <v>1.8903988741624482E-5</v>
+        <v>6.1627003297695804E-6</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated industrial cost efficiency indst/ctieppuesos
</commit_message>
<xml_diff>
--- a/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
+++ b/InputData/indst/CtIEPpUESoS/Cost to Impl Eff Policy per Unit E Saved or Shifted.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\indst\CtIEPpUESoS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\us-eps\InputData\indst\CtIEPpUESoS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A4E9C2A-F4CA-4670-8026-422A565CD66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEAEDC2E-6B42-4CB5-AFA1-775DD85ABCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="780" windowWidth="15900" windowHeight="22005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11100" yWindow="1140" windowWidth="16605" windowHeight="15210" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="early retirement" sheetId="4" r:id="rId2"/>
-    <sheet name="cogen and WHR + eqpt stds" sheetId="6" r:id="rId3"/>
-    <sheet name="med and high temp fuel shifting" sheetId="5" r:id="rId4"/>
-    <sheet name="low temp fuel type shifting" sheetId="8" r:id="rId5"/>
-    <sheet name="CtIEPpUESoS" sheetId="3" r:id="rId6"/>
+    <sheet name="cogen and WHR" sheetId="6" r:id="rId3"/>
+    <sheet name="efficiency" sheetId="10" r:id="rId4"/>
+    <sheet name="med and high temp fuel shifting" sheetId="5" r:id="rId5"/>
+    <sheet name="low temp fuel type shifting" sheetId="8" r:id="rId6"/>
+    <sheet name="substitute fuels for coal" sheetId="9" r:id="rId7"/>
+    <sheet name="CtIEPpUESoS" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -80,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="172">
   <si>
     <t>Source:</t>
   </si>
@@ -217,12 +219,6 @@
     <t>All costs are per BTU of energy saved or shifted per year.  That is, it is the cost to buy equipment that</t>
   </si>
   <si>
-    <t>cogeneration and WHR, equipment standards: total cost</t>
-  </si>
-  <si>
-    <t>cogeneration and WHR, equipment standards: annual energy savings</t>
-  </si>
-  <si>
     <t>Reinventing Fire</t>
   </si>
   <si>
@@ -247,9 +243,6 @@
     <t>Cost per Unit Energy Saved Annually ($/BTU)</t>
   </si>
   <si>
-    <t>efficiency technology</t>
-  </si>
-  <si>
     <t>The graph used appears below.  To correspond to the total energy savings found above, we want to use the set of pink bars that</t>
   </si>
   <si>
@@ -518,6 +511,93 @@
   </si>
   <si>
     <t>Therefore, the capital cost per unit energy saved (not per unit energy delivered) is:</t>
+  </si>
+  <si>
+    <t>Substitute Other Fuels for Coal</t>
+  </si>
+  <si>
+    <t>We estimate the cost of converting coal equipment to use other fuel types</t>
+  </si>
+  <si>
+    <t>via the conversion of coal-fired biolers to natural gas, because of the</t>
+  </si>
+  <si>
+    <t>availability of data.</t>
+  </si>
+  <si>
+    <t>Typical Pulverized Coal to Natural Gas Conversions</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Cost per Unit Capacity ($/kW)</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>Industrial Boiler Capacity Factor</t>
+  </si>
+  <si>
+    <t>Hours per Year</t>
+  </si>
+  <si>
+    <t>Investment Cost per Unit Annual Energy Converted ($/kWh)</t>
+  </si>
+  <si>
+    <t>Investment per Unit Energy Converted ($/BTU)</t>
+  </si>
+  <si>
+    <t>substitute other fuels for coal: conversion costs per unit capacity</t>
+  </si>
+  <si>
+    <t>Babcock and Wilcox</t>
+  </si>
+  <si>
+    <t>Natural Gas Conversions of Existing Coal-Fired Boilers</t>
+  </si>
+  <si>
+    <t>http://www.babcock.com/library/Documents/MS-14.pdf</t>
+  </si>
+  <si>
+    <t>Page 2, "Financial Considerations," paragraph 1</t>
+  </si>
+  <si>
+    <t>Tbtu/year</t>
+  </si>
+  <si>
+    <t>We assume outlays are uniform in each year and that savings also accrue uniformly.</t>
+  </si>
+  <si>
+    <t>McKinsey used a 7 percent discount rate in their main scenario</t>
+  </si>
+  <si>
+    <t>2009 to 2012 USD</t>
+  </si>
+  <si>
+    <t>cogeneration and WHR: total cost</t>
+  </si>
+  <si>
+    <t>cogeneration and WHR: annual energy savings</t>
+  </si>
+  <si>
+    <t>McKinsey</t>
+  </si>
+  <si>
+    <t>Unlocking Energy Efficiency in the U.S. Economy</t>
+  </si>
+  <si>
+    <t>https://www.sallan.org/pdf-docs/MCKINSEY_US_energy_efficiency.pdf</t>
+  </si>
+  <si>
+    <t>Tables 15 and 16</t>
   </si>
 </sst>
 </file>
@@ -627,7 +707,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -660,6 +740,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,7 +833,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
@@ -833,6 +919,29 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Body: normal cell" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -904,6 +1013,99 @@
         <a:xfrm>
           <a:off x="0" y="4581525"/>
           <a:ext cx="7620000" cy="5429250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>129654</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63777A4A-2F0B-9B40-B441-F44633B09A2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1905000"/>
+          <a:ext cx="4000500" cy="3558654"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>237614</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104245</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BE7B3D1-B516-269F-941C-3CC5A2176C1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4076700" y="1962150"/>
+          <a:ext cx="4085714" cy="4238095"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1236,86 +1438,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="81.7109375" customWidth="1"/>
+    <col min="4" max="4" width="56.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2013</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" s="54">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" s="25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8" s="25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11" s="25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>2011</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D12" s="54">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D13" s="25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>27</v>
       </c>
+      <c r="D15" s="25" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -1330,32 +1571,32 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="25" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1365,7 +1606,7 @@
     </row>
     <row r="28" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
@@ -1373,12 +1614,12 @@
     </row>
     <row r="30" spans="2:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="2:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="2:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -1388,12 +1629,12 @@
     </row>
     <row r="33" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1406,12 +1647,12 @@
     </row>
     <row r="38" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -1419,12 +1660,12 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1439,43 +1680,43 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1483,7 +1724,7 @@
         <v>0.98699999999999999</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -1491,12 +1732,12 @@
         <v>1.0549999999999999</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1505,9 +1746,10 @@
     <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B21" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B34" r:id="rId4" xr:uid="{6376C4F0-B677-4CE5-9217-A9D26BE45B75}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{1577CB84-3B18-4B4B-9741-3317554DFE0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1515,7 +1757,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1670,9 +1914,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1681,11 +1927,14 @@
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1693,13 +1942,13 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="10"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B4" s="21">
         <f>2.4*10^15</f>
@@ -1707,45 +1956,39 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="21">
-        <f>2.3*10^15</f>
-        <v>2300000000000000</v>
-      </c>
+      <c r="B5" s="21"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1758,40 +2001,40 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>34</v>
       </c>
@@ -1800,23 +2043,23 @@
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
         <v>62</v>
       </c>
-      <c r="D24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B25" s="17">
         <v>114</v>
@@ -1833,42 +2076,29 @@
         <v>54807017543.85965</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="17">
-        <v>114</v>
-      </c>
-      <c r="C26" s="5">
-        <v>5</v>
-      </c>
-      <c r="D26" s="18">
-        <f>284*10^9</f>
-        <v>284000000000</v>
-      </c>
-      <c r="E26" s="22">
-        <f>(C26/B26)*D26</f>
-        <v>12456140350.877192</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="17"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="17"/>
       <c r="B27" s="5"/>
       <c r="C27" s="18"/>
       <c r="D27" s="22"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="24"/>
       <c r="C28" s="18"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B29" s="23">
         <f>E25/B4</f>
@@ -1877,16 +2107,11 @@
       <c r="C29" s="18"/>
       <c r="D29" s="22"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="23">
-        <f>E26/B5</f>
-        <v>5.4157131960335617E-6</v>
-      </c>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="25"/>
       <c r="C30" s="18"/>
       <c r="D30" s="22"/>
+      <c r="G30" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1896,10 +2121,437 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131020BD-F268-461F-B03F-7101039E9E7B}">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25">
+        <v>2009</v>
+      </c>
+      <c r="C1" s="25">
+        <v>2010</v>
+      </c>
+      <c r="D1" s="25">
+        <v>2011</v>
+      </c>
+      <c r="E1" s="25">
+        <v>2012</v>
+      </c>
+      <c r="F1" s="25">
+        <v>2013</v>
+      </c>
+      <c r="G1" s="25">
+        <v>2014</v>
+      </c>
+      <c r="H1" s="25">
+        <v>2015</v>
+      </c>
+      <c r="I1" s="25">
+        <v>2016</v>
+      </c>
+      <c r="J1" s="25">
+        <v>2017</v>
+      </c>
+      <c r="K1" s="25">
+        <v>2018</v>
+      </c>
+      <c r="L1" s="25">
+        <v>2019</v>
+      </c>
+      <c r="M1" s="25">
+        <v>2020</v>
+      </c>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="20">
+        <f>NPV(0.07,B2:M2)</f>
+        <v>79000000000.000015</v>
+      </c>
+      <c r="B2" s="20">
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="C2" s="20">
+        <f>B2</f>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="D2" s="20">
+        <f t="shared" ref="D2:M2" si="0">C2</f>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="E2" s="20">
+        <f t="shared" si="0"/>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="F2" s="20">
+        <f t="shared" si="0"/>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="G2" s="20">
+        <f t="shared" si="0"/>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="H2" s="20">
+        <f t="shared" si="0"/>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="I2" s="20">
+        <f t="shared" si="0"/>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="J2" s="20">
+        <f t="shared" si="0"/>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="K2" s="20">
+        <f t="shared" si="0"/>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="L2" s="20">
+        <f t="shared" si="0"/>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="M2" s="20">
+        <f t="shared" si="0"/>
+        <v>9946257103.7466221</v>
+      </c>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="25">
+        <f>51+28</f>
+        <v>79</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25">
+        <f>M4/COUNT(B1:M1)</f>
+        <v>201.66666666666666</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25">
+        <f>1550+870</f>
+        <v>2420</v>
+      </c>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="20">
+        <f>B2/(B4*1000000000000)*Q5</f>
+        <v>5.2772702980209352E-5</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q5">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
@@ -1914,43 +2566,43 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C8" s="31">
         <v>25</v>
@@ -1958,10 +2610,10 @@
     </row>
     <row r="9" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C9" s="32">
         <v>0.05</v>
@@ -1969,10 +2621,10 @@
     </row>
     <row r="10" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C10" s="33">
         <v>6.5242598122280206</v>
@@ -1981,10 +2633,10 @@
     </row>
     <row r="11" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C11" s="39">
         <v>6.3954140084752677E-3</v>
@@ -1992,10 +2644,10 @@
     </row>
     <row r="12" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C12" s="39">
         <v>52.826854199999993</v>
@@ -2004,29 +2656,29 @@
     <row r="13" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C16" s="34">
         <v>53860</v>
@@ -2037,10 +2689,10 @@
     </row>
     <row r="17" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C17" s="32">
         <v>1</v>
@@ -2051,10 +2703,10 @@
     </row>
     <row r="18" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C18" s="36">
         <v>3.3475000000000001</v>
@@ -2065,10 +2717,10 @@
     </row>
     <row r="19" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C19" s="37">
         <v>5280</v>
@@ -2079,10 +2731,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C20" s="37">
         <f>C18*C19</f>
@@ -2100,7 +2752,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B23" s="8"/>
     </row>
@@ -2112,7 +2764,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2120,7 +2772,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="25"/>
@@ -2128,22 +2780,22 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D30" s="25"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C31" s="31">
         <v>25</v>
@@ -2152,10 +2804,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C32" s="32">
         <v>0.05</v>
@@ -2164,10 +2816,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C33" s="33">
         <f>C10</f>
@@ -2177,10 +2829,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C34" s="34">
         <v>44</v>
@@ -2189,10 +2841,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C35" s="34">
         <v>34</v>
@@ -2201,10 +2853,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C36" s="34">
         <v>21</v>
@@ -2213,10 +2865,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C37" s="34">
         <v>15</v>
@@ -2225,10 +2877,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C38" s="34">
         <v>4</v>
@@ -2243,7 +2895,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -2251,24 +2903,24 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C42" s="34">
         <v>87540</v>
@@ -2279,10 +2931,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C43" s="34">
         <f>C42*1.5</f>
@@ -2294,10 +2946,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C44" s="32">
         <f>D44</f>
@@ -2309,10 +2961,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C45" s="36">
         <v>3.3475000000000001</v>
@@ -2323,10 +2975,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C46" s="37">
         <v>5280</v>
@@ -2337,10 +2989,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C47" s="37">
         <f>C45*C46</f>
@@ -2353,7 +3005,7 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -2368,15 +3020,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70154B78-0E9B-4A9B-9D3C-65AF6790BABC}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="25" customWidth="1"/>
     <col min="2" max="3" width="19.140625" style="25" customWidth="1"/>
@@ -2386,23 +3038,23 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="42" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C3" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="40" t="s">
         <v>131</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B4" s="25">
         <v>56603</v>
@@ -2417,7 +3069,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B5" s="25">
         <v>25717</v>
@@ -2432,7 +3084,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B6" s="25">
         <v>60507</v>
@@ -2447,7 +3099,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B7" s="25">
         <f>AVERAGE(B4:B6)</f>
@@ -2464,27 +3116,27 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2494,7 +3146,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -2510,24 +3162,178 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586C6099-D878-4CA6-905E-BCE566C93FAD}">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="25" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="42"/>
+      <c r="B5" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="42"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="C6" s="47"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="49"/>
+      <c r="C7" s="47"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="47"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="50">
+        <v>50</v>
+      </c>
+      <c r="C9" s="47"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="50">
+        <v>75</v>
+      </c>
+      <c r="C10" s="47"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="52">
+        <f>AVERAGE(B9:B10)</f>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <f>24*365</f>
+        <v>8760</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="53">
+        <f>B11/(A17*A14)</f>
+        <v>1.5180219566695814E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <f>2.93*10^-4</f>
+        <v>2.9300000000000002E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <f>A20*A23</f>
+        <v>4.4478043330418734E-6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B1" s="27">
         <v>2018</v>
@@ -2907,7 +3713,7 @@
         <v>38</v>
       </c>
       <c r="B4" s="20">
-        <f>'cogen and WHR + eqpt stds'!B29*About!$A$58</f>
+        <f>'cogen and WHR'!B29*About!$A$58</f>
         <v>2.4092251461988303E-5</v>
       </c>
       <c r="C4" s="20">
@@ -3044,278 +3850,278 @@
         <v>39</v>
       </c>
       <c r="B5" s="20">
-        <f>'cogen and WHR + eqpt stds'!B30*About!$A$58</f>
-        <v>5.7135774218154072E-6</v>
+        <f>efficiency!B5</f>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="C5" s="20">
         <f t="shared" si="1"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="D5" s="20">
         <f t="shared" si="1"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="E5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="F5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="G5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="H5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="I5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="J5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="K5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="L5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="M5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="N5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="O5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="P5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="Q5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="R5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="S5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="T5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="U5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="V5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="W5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="X5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="Y5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="Z5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="AA5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="AB5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="AC5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="AD5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="AE5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="AF5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="AG5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
       <c r="AH5" s="20">
         <f t="shared" si="0"/>
-        <v>5.7135774218154072E-6</v>
+        <v>5.2772702980209352E-5</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B6" s="20">
-        <f>AVERAGE('med and high temp fuel shifting'!A24,'med and high temp fuel shifting'!A50)*About!$A$58</f>
-        <v>4.8732001210763347E-6</v>
+        <f>'med and high temp fuel shifting'!$A$50</f>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="C6" s="20">
         <f t="shared" si="1"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="D6" s="20">
         <f t="shared" si="1"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="E6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="F6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="G6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="H6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="I6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="J6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="K6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="L6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="M6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="N6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="O6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="P6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="Q6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="R6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="S6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="T6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="U6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="V6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="W6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="X6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="Y6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="Z6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="AA6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="AB6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="AC6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="AD6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="AE6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="AF6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="AG6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
       <c r="AH6" s="20">
         <f t="shared" si="0"/>
-        <v>4.8732001210763347E-6</v>
+        <v>6.1910177201439334E-6</v>
       </c>
     </row>
     <row r="7" spans="1:34" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B7" s="44">
         <f>'low temp fuel type shifting'!A18</f>
@@ -3454,7 +4260,7 @@
       <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="20">
         <v>0</v>
       </c>
       <c r="C8" s="28">

</xml_diff>